<commit_message>
linpack: updated Excel results with KVM tuned bar
</commit_message>
<xml_diff>
--- a/linpack/results/linpack.xlsx
+++ b/linpack/results/linpack.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33520" windowHeight="20560" tabRatio="500"/>
+    <workbookView xWindow="3260" yWindow="1320" windowWidth="19100" windowHeight="18520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Native</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>SD</t>
+  </si>
+  <si>
+    <t>KVM untuned</t>
+  </si>
+  <si>
+    <t>KVM tuned</t>
   </si>
 </sst>
 </file>
@@ -100,8 +106,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -132,7 +144,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -144,6 +156,9 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -155,6 +170,9 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -284,11 +302,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2119510808"/>
-        <c:axId val="-2119507832"/>
+        <c:axId val="2065991960"/>
+        <c:axId val="2064363448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2119510808"/>
+        <c:axId val="2065991960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -297,7 +315,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119507832"/>
+        <c:crossAx val="2064363448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -305,7 +323,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2119507832"/>
+        <c:axId val="2064363448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -340,7 +358,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119510808"/>
+        <c:crossAx val="2065991960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -399,10 +417,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$E$30:$G$30</c:f>
+                <c:f>Sheet1!$E$30:$H$30</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
+                  <c:ptCount val="4"/>
                   <c:pt idx="0">
                     <c:v>1.133385878389758</c:v>
                   </c:pt>
@@ -411,16 +429,19 @@
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>7.565772761765098</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.450492583151591</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$E$31:$G$31</c:f>
+                <c:f>Sheet1!$E$31:$H$31</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
+                  <c:ptCount val="4"/>
                   <c:pt idx="0">
                     <c:v>1.133385878389758</c:v>
                   </c:pt>
@@ -429,6 +450,9 @@
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>7.565772761765098</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.450492583151591</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -436,9 +460,9 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$18:$G$18</c:f>
+              <c:f>Sheet1!$E$18:$H$18</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Native</c:v>
                 </c:pt>
@@ -446,17 +470,20 @@
                   <c:v>Docker</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>KVM</c:v>
+                  <c:v>KVM untuned</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>KVM tuned</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$29:$G$29</c:f>
+              <c:f>Sheet1!$E$29:$H$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>290.82864</c:v>
                 </c:pt>
@@ -465,6 +492,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>130.28326</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>284.19874</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -479,11 +509,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2137657288"/>
-        <c:axId val="2082812488"/>
+        <c:axId val="2071627864"/>
+        <c:axId val="2071733784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2137657288"/>
+        <c:axId val="2071627864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -492,7 +522,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082812488"/>
+        <c:crossAx val="2071733784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -500,7 +530,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2082812488"/>
+        <c:axId val="2071733784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,7 +560,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137657288"/>
+        <c:crossAx val="2071627864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -938,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A16:G31"/>
+  <dimension ref="A16:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -961,7 +991,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="18">
+    <row r="17" spans="1:8" ht="18">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
         <v>4</v>
@@ -974,7 +1004,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="18">
+    <row r="18" spans="1:8" ht="18">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -994,10 +1024,13 @@
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="18">
+        <v>9</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="18">
       <c r="A19" s="1"/>
       <c r="E19" s="1">
         <v>291.5018</v>
@@ -1008,8 +1041,11 @@
       <c r="G19" s="1">
         <v>132.70670000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="18">
+      <c r="H19">
+        <v>283.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="18">
       <c r="A20" s="1"/>
       <c r="E20" s="1">
         <v>291.35109999999997</v>
@@ -1020,8 +1056,11 @@
       <c r="G20" s="1">
         <v>132.9015</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="18">
+      <c r="H20">
+        <v>286.10809999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18">
       <c r="A21" s="1"/>
       <c r="E21" s="1">
         <v>290.2783</v>
@@ -1032,8 +1071,11 @@
       <c r="G21" s="1">
         <v>132.86070000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="18">
+      <c r="H21" s="1">
+        <v>282.76049999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18">
       <c r="A22" s="1"/>
       <c r="E22" s="1">
         <v>292.18740000000003</v>
@@ -1044,8 +1086,11 @@
       <c r="G22" s="1">
         <v>132.614</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="18">
+      <c r="H22">
+        <v>285.90820000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="18">
       <c r="A23" s="1"/>
       <c r="E23" s="1">
         <v>290.20600000000002</v>
@@ -1056,8 +1101,11 @@
       <c r="G23" s="1">
         <v>132.6397</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="18">
+      <c r="H23">
+        <v>282.30180000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18">
       <c r="A24" s="1"/>
       <c r="E24" s="1">
         <v>289.53500000000003</v>
@@ -1068,8 +1116,11 @@
       <c r="G24" s="1">
         <v>132.5018</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="18">
+      <c r="H24">
+        <v>284.2944</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="18">
       <c r="A25" s="1"/>
       <c r="E25" s="1">
         <v>291.82440000000003</v>
@@ -1080,8 +1131,11 @@
       <c r="G25" s="1">
         <v>132.65459999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="18">
+      <c r="H25">
+        <v>284.279</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18">
       <c r="A26" s="1"/>
       <c r="E26" s="1">
         <v>289.51350000000002</v>
@@ -1092,8 +1146,11 @@
       <c r="G26" s="1">
         <v>108.7559</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="18">
+      <c r="H26">
+        <v>285.9597</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18">
       <c r="A27" s="1"/>
       <c r="E27" s="1">
         <v>289.55220000000003</v>
@@ -1104,8 +1161,11 @@
       <c r="G27" s="1">
         <v>132.3587</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="18">
+      <c r="H27">
+        <v>282.322</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18">
       <c r="A28" s="1"/>
       <c r="E28" s="1">
         <v>292.33670000000001</v>
@@ -1116,8 +1176,11 @@
       <c r="G28" s="1">
         <v>132.839</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="18">
+      <c r="H28">
+        <v>284.06369999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="18">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
@@ -1126,7 +1189,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="C29" s="1" t="e">
-        <f t="shared" ref="C29:G29" si="0">AVERAGE(C19:C28)</f>
+        <f t="shared" ref="C29:H29" si="0">AVERAGE(C19:C28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D29" s="1" t="e">
@@ -1145,8 +1208,12 @@
         <f t="shared" si="0"/>
         <v>130.28325999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="18">
+      <c r="H29" s="1">
+        <f t="shared" si="0"/>
+        <v>284.19873999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="18">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -1155,7 +1222,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="C30" s="1" t="e">
-        <f t="shared" ref="C30:G30" si="1">STDEV(C19:C28)</f>
+        <f t="shared" ref="C30:H30" si="1">STDEV(C19:C28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D30" s="1" t="e">
@@ -1174,8 +1241,12 @@
         <f t="shared" si="1"/>
         <v>7.5657727617650981</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="18">
+      <c r="H30" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4504925831515911</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -1184,7 +1255,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="C31" s="1" t="e">
-        <f t="shared" ref="C31:G31" si="2">STDEV(C19:C28)</f>
+        <f t="shared" ref="C31:H31" si="2">STDEV(C19:C28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D31" s="1" t="e">
@@ -1202,6 +1273,10 @@
       <c r="G31" s="1">
         <f t="shared" si="2"/>
         <v>7.5657727617650981</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="2"/>
+        <v>1.4504925831515911</v>
       </c>
     </row>
   </sheetData>

</xml_diff>